<commit_message>
Application deboarding code added
</commit_message>
<xml_diff>
--- a/input-data/inputFiles/InputData.xlsx
+++ b/input-data/inputFiles/InputData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\APathrut\eclipse-workspace\e2colitmus\E2CO%20Automation\input-data\inputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69AEB3FA-811F-4ACE-BBA6-B0B588F01222}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63A54EA2-5A68-4A66-9D43-3F34EE3B93EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="7" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="118">
   <si>
     <t>Version</t>
   </si>
@@ -261,9 +261,6 @@
     <t>versionDelete</t>
   </si>
   <si>
-    <t>artifact0305</t>
-  </si>
-  <si>
     <t>artifact0304</t>
   </si>
   <si>
@@ -294,18 +291,9 @@
     <t>instanceId</t>
   </si>
   <si>
-    <t>alpineapp212</t>
-  </si>
-  <si>
-    <t>v64036b586000010</t>
-  </si>
-  <si>
     <t>1.0</t>
   </si>
   <si>
-    <t>64036c6e5000009</t>
-  </si>
-  <si>
     <t>domainName</t>
   </si>
   <si>
@@ -381,20 +369,29 @@
     <t>ZoneName</t>
   </si>
   <si>
-    <t>alpineapp1658</t>
-  </si>
-  <si>
     <t>ApplicationNameFrProvision</t>
   </si>
   <si>
     <t>ApplicationNameFrDeProvision</t>
+  </si>
+  <si>
+    <t>j6425faa1e000010</t>
+  </si>
+  <si>
+    <t>6425ff74d000003</t>
+  </si>
+  <si>
+    <t>artifact0310</t>
+  </si>
+  <si>
+    <t>ApplicationNmFrDeboard</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -415,6 +412,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF8F8F8F"/>
+      <name val="Ubuntu"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -466,7 +475,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -488,6 +497,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -771,7 +783,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D45AE27-C122-4BD5-BBB5-8CE7C7A56A51}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -789,33 +801,33 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>69</v>
@@ -824,10 +836,10 @@
         <v>28</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>69</v>
@@ -841,7 +853,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>69</v>
@@ -850,10 +862,10 @@
         <v>28</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>69</v>
@@ -867,7 +879,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>69</v>
@@ -876,10 +888,10 @@
         <v>28</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>69</v>
@@ -893,7 +905,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>69</v>
@@ -902,10 +914,10 @@
         <v>28</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F5" s="8" t="s">
         <v>69</v>
@@ -1207,7 +1219,7 @@
         <v>53</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>26</v>
@@ -1288,10 +1300,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DC37D6C-9FD6-4975-A3E4-794B22D0C261}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1305,9 +1317,10 @@
     <col min="9" max="9" width="24.5546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="26.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>37</v>
       </c>
@@ -1333,21 +1346,24 @@
         <v>43</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="L1" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>44</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>76</v>
+        <v>116</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>46</v>
@@ -1356,33 +1372,36 @@
         <v>48</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>51</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="H2" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>116</v>
+      <c r="I2" s="11" t="s">
+        <v>97</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+        <v>96</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="L2" s="12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>45</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>47</v>
@@ -1405,10 +1424,12 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1464,7 +1485,7 @@
         <v>64</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -1551,7 +1572,7 @@
         <v>68</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>69</v>
@@ -1569,7 +1590,7 @@
         <v>30</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -1586,7 +1607,7 @@
         <v>72</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>69</v>
@@ -1604,12 +1625,12 @@
         <v>60</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B6" s="6">
         <v>1234</v>
@@ -1621,22 +1642,22 @@
         <v>72</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="K6" s="1">
         <v>1234</v>
@@ -1682,13 +1703,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>80</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -1696,7 +1717,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B2" s="1">
         <v>2</v>
@@ -1705,7 +1726,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1718,7 +1739,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1731,30 +1752,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>90</v>
+      <c r="D2" s="13" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
My applications added more validations
</commit_message>
<xml_diff>
--- a/input-data/inputFiles/InputData.xlsx
+++ b/input-data/inputFiles/InputData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\APathrut\eclipse-workspace\e2colitmus\E2CO%20Automation\input-data\inputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63A54EA2-5A68-4A66-9D43-3F34EE3B93EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35D0C1EB-33E4-49DD-8C4A-5668CA060A62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="120">
   <si>
     <t>Version</t>
   </si>
@@ -385,6 +385,12 @@
   </si>
   <si>
     <t>ApplicationNmFrDeboard</t>
+  </si>
+  <si>
+    <t>artifact0311</t>
+  </si>
+  <si>
+    <t>appdemo213</t>
   </si>
 </sst>
 </file>
@@ -1300,10 +1306,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DC37D6C-9FD6-4975-A3E4-794B22D0C261}">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView tabSelected="1" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1398,33 +1404,71 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>76</v>
+        <v>118</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>50</v>
+        <v>119</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>51</v>
       </c>
       <c r="G3" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="K3" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="L3" s="11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H4" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
some changes in excel sheet done
</commit_message>
<xml_diff>
--- a/input-data/inputFiles/InputData.xlsx
+++ b/input-data/inputFiles/InputData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\APathrut\eclipse-workspace\e2colitmus\E2CO%20Automation\input-data\inputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35D0C1EB-33E4-49DD-8C4A-5668CA060A62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{372006C8-C68D-43CF-8AE9-8816ABD62F43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="118">
   <si>
     <t>Version</t>
   </si>
@@ -300,13 +300,7 @@
     <t>admin0703</t>
   </si>
   <si>
-    <t>Solapur</t>
-  </si>
-  <si>
     <t>dev0703</t>
-  </si>
-  <si>
-    <t>Pune</t>
   </si>
   <si>
     <t>dev0704</t>
@@ -440,7 +434,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -463,25 +457,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -500,10 +481,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
@@ -807,33 +784,33 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>69</v>
@@ -842,10 +819,10 @@
         <v>28</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>69</v>
@@ -859,7 +836,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>69</v>
@@ -868,10 +845,10 @@
         <v>28</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>69</v>
@@ -885,7 +862,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>69</v>
@@ -894,10 +871,10 @@
         <v>28</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>69</v>
@@ -911,7 +888,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>69</v>
@@ -920,10 +897,10 @@
         <v>28</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F5" s="8" t="s">
         <v>69</v>
@@ -961,19 +938,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -983,8 +961,11 @@
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -994,8 +975,11 @@
       <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" s="1">
+        <v>12345</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1005,8 +989,11 @@
       <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" s="1">
+        <v>67890</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1016,8 +1003,11 @@
       <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4" s="1">
+        <v>21223</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1027,8 +1017,11 @@
       <c r="C5" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5" s="1">
+        <v>41423</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -1038,34 +1031,7 @@
       <c r="C6" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
-        <v>12345</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
-        <v>67890</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
-        <v>21223</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="1">
-        <v>41423</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="1">
+      <c r="D6" s="1">
         <v>31323</v>
       </c>
     </row>
@@ -1076,10 +1042,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0442710-9812-4BB8-A29F-019BB15B721A}">
-  <dimension ref="A1:T7"/>
+  <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="V11" sqref="V11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1096,7 +1062,7 @@
     <col min="21" max="21" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1157,8 +1123,11 @@
       <c r="T1" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U1" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>52</v>
       </c>
@@ -1219,13 +1188,16 @@
       <c r="T2" s="1">
         <v>-34.703800000000001</v>
       </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U2" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>26</v>
@@ -1281,19 +1253,7 @@
       <c r="T3" s="1">
         <v>-34.703800000000001</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+      <c r="U3" s="1" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1309,7 +1269,7 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1348,20 +1308,20 @@
       <c r="G1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="4" t="s">
         <v>43</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>113</v>
-      </c>
       <c r="L1" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
@@ -1369,7 +1329,7 @@
         <v>44</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>46</v>
@@ -1378,28 +1338,28 @@
         <v>48</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>51</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="I2" s="11" t="s">
-        <v>97</v>
+      <c r="I2" s="10" t="s">
+        <v>95</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="K2" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="L2" s="12" t="s">
-        <v>97</v>
+        <v>94</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -1407,7 +1367,7 @@
         <v>44</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>46</v>
@@ -1416,28 +1376,28 @@
         <v>48</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>51</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="I3" s="11" t="s">
-        <v>119</v>
+      <c r="I3" s="10" t="s">
+        <v>117</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="K3" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="L3" s="11" t="s">
-        <v>119</v>
+        <v>94</v>
+      </c>
+      <c r="K3" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -1462,7 +1422,7 @@
       <c r="G4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="4" t="s">
         <v>28</v>
       </c>
       <c r="I4" s="1"/>
@@ -1482,7 +1442,7 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1633,8 +1593,8 @@
       <c r="J4" s="4">
         <v>30</v>
       </c>
-      <c r="K4" s="3" t="s">
-        <v>89</v>
+      <c r="K4" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -1651,7 +1611,7 @@
         <v>72</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>69</v>
@@ -1668,13 +1628,13 @@
       <c r="J5" s="6">
         <v>60</v>
       </c>
-      <c r="K5" s="3" t="s">
-        <v>91</v>
+      <c r="K5" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B6" s="6">
         <v>1234</v>
@@ -1686,22 +1646,22 @@
         <v>72</v>
       </c>
       <c r="E6" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>94</v>
-      </c>
       <c r="G6" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K6" s="1">
         <v>1234</v>
@@ -1809,17 +1769,17 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>114</v>
+      <c r="A2" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>112</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D2" s="13" t="s">
-        <v>115</v>
+      <c r="D2" s="11" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new code more scenarios added
</commit_message>
<xml_diff>
--- a/input-data/inputFiles/InputData.xlsx
+++ b/input-data/inputFiles/InputData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://capgemini-my.sharepoint.com/personal/abhishek-chidanand_pathrut_capgemini_com/Documents/Desktop/E2CO PROJECT/Automation/E2COAutomation/E2CO%20Automation/input-data/inputFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{372006C8-C68D-43CF-8AE9-8816ABD62F43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6F9F8EB5-029C-406A-AD32-C4678D00EA02}"/>
+  <xr:revisionPtr revIDLastSave="57" documentId="13_ncr:1_{372006C8-C68D-43CF-8AE9-8816ABD62F43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C6500A4D-EAD1-45A2-A6CB-09800A8B03B6}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="7" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="122">
   <si>
     <t>Version</t>
   </si>
@@ -108,12 +108,6 @@
     <t>Longitude</t>
   </si>
   <si>
-    <t>SouthZone</t>
-  </si>
-  <si>
-    <t>India</t>
-  </si>
-  <si>
     <t>Low</t>
   </si>
   <si>
@@ -171,9 +165,6 @@
     <t>VM</t>
   </si>
   <si>
-    <t>alpine1</t>
-  </si>
-  <si>
     <t>fedora</t>
   </si>
   <si>
@@ -315,76 +306,97 @@
     <t>dev@1234</t>
   </si>
   <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>DomainName</t>
+  </si>
+  <si>
+    <t>admin212</t>
+  </si>
+  <si>
+    <t>dev212</t>
+  </si>
+  <si>
+    <t>admin17</t>
+  </si>
+  <si>
+    <t>dev17</t>
+  </si>
+  <si>
+    <t>OldPassword</t>
+  </si>
+  <si>
+    <t>NewPassword</t>
+  </si>
+  <si>
+    <t>RetypeNewPassword</t>
+  </si>
+  <si>
+    <t>domainname</t>
+  </si>
+  <si>
+    <t>Admin@12345</t>
+  </si>
+  <si>
+    <t>UNRestPass</t>
+  </si>
+  <si>
+    <t>ZoneName</t>
+  </si>
+  <si>
+    <t>ApplicationNameFrProvision</t>
+  </si>
+  <si>
+    <t>ApplicationNameFrDeProvision</t>
+  </si>
+  <si>
+    <t>artifact0310</t>
+  </si>
+  <si>
+    <t>ApplicationNmFrDeboard</t>
+  </si>
+  <si>
+    <t>artifact0311</t>
+  </si>
+  <si>
+    <t>appdemo213</t>
+  </si>
+  <si>
+    <t>EastZone</t>
+  </si>
+  <si>
+    <t>IN</t>
+  </si>
+  <si>
+    <t>marioapp0005</t>
+  </si>
+  <si>
+    <t>64813a8d2000005</t>
+  </si>
+  <si>
+    <t>f6480bac6c000010</t>
+  </si>
+  <si>
+    <t>alpine</t>
+  </si>
+  <si>
+    <t>EdgeForDetails</t>
+  </si>
+  <si>
+    <t>edge1</t>
+  </si>
+  <si>
+    <t>edge2</t>
+  </si>
+  <si>
+    <t>appdemo214</t>
+  </si>
+  <si>
     <t>NorthZone</t>
-  </si>
-  <si>
-    <t>appdemo212</t>
-  </si>
-  <si>
-    <t>UserName</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>DomainName</t>
-  </si>
-  <si>
-    <t>admin212</t>
-  </si>
-  <si>
-    <t>dev212</t>
-  </si>
-  <si>
-    <t>admin17</t>
-  </si>
-  <si>
-    <t>dev17</t>
-  </si>
-  <si>
-    <t>OldPassword</t>
-  </si>
-  <si>
-    <t>NewPassword</t>
-  </si>
-  <si>
-    <t>RetypeNewPassword</t>
-  </si>
-  <si>
-    <t>domainname</t>
-  </si>
-  <si>
-    <t>Admin@12345</t>
-  </si>
-  <si>
-    <t>UNRestPass</t>
-  </si>
-  <si>
-    <t>ZoneName</t>
-  </si>
-  <si>
-    <t>ApplicationNameFrProvision</t>
-  </si>
-  <si>
-    <t>ApplicationNameFrDeProvision</t>
-  </si>
-  <si>
-    <t>j6425faa1e000010</t>
-  </si>
-  <si>
-    <t>6425ff74d000003</t>
-  </si>
-  <si>
-    <t>artifact0310</t>
-  </si>
-  <si>
-    <t>ApplicationNmFrDeboard</t>
-  </si>
-  <si>
-    <t>artifact0311</t>
-  </si>
-  <si>
-    <t>appdemo213</t>
   </si>
 </sst>
 </file>
@@ -766,8 +778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D45AE27-C122-4BD5-BBB5-8CE7C7A56A51}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -784,132 +796,132 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>69</v>
+        <v>102</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>107</v>
+        <v>66</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>107</v>
+        <v>66</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="F5" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="1" t="s">
+      <c r="G5" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="E5" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>107</v>
-      </c>
       <c r="H5" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -962,7 +974,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -1042,9 +1054,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0442710-9812-4BB8-A29F-019BB15B721A}">
-  <dimension ref="A1:U3"/>
+  <dimension ref="A1:V3"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
+    <sheetView zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
       <selection activeCell="V11" sqref="V11"/>
     </sheetView>
   </sheetViews>
@@ -1059,10 +1071,11 @@
     <col min="10" max="10" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14" customWidth="1"/>
+    <col min="22" max="22" width="13.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1124,48 +1137,51 @@
         <v>24</v>
       </c>
       <c r="U1" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="F2" s="1">
         <v>10</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="L2" s="1">
         <v>404</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="N2" s="1">
         <v>1</v>
@@ -1180,7 +1196,7 @@
         <v>2</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="S2" s="1">
         <v>12.4168</v>
@@ -1189,48 +1205,51 @@
         <v>-34.703800000000001</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="F3" s="1">
         <v>40</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="L3" s="1">
         <v>404</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="N3" s="1">
         <v>1</v>
@@ -1245,7 +1264,7 @@
         <v>2</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="S3" s="1">
         <v>12.4168</v>
@@ -1254,7 +1273,10 @@
         <v>-34.703800000000001</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -1268,8 +1290,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DC37D6C-9FD6-4975-A3E4-794B22D0C261}">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1278,7 +1300,7 @@
     <col min="2" max="2" width="13.88671875" customWidth="1"/>
     <col min="3" max="4" width="35.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" customWidth="1"/>
     <col min="8" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="24.5546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
@@ -1288,142 +1310,142 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>41</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>8</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>46</v>
+        <v>116</v>
       </c>
       <c r="D2" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>51</v>
-      </c>
       <c r="G2" s="4" t="s">
-        <v>94</v>
+        <v>121</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>94</v>
+        <v>120</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>121</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>95</v>
+        <v>120</v>
       </c>
       <c r="L2" s="10" t="s">
-        <v>95</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>46</v>
-      </c>
       <c r="D3" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>51</v>
-      </c>
       <c r="G3" s="4" t="s">
-        <v>94</v>
+        <v>121</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>94</v>
+        <v>110</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>121</v>
       </c>
       <c r="K3" s="10" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="L3" s="10" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>50</v>
-      </c>
       <c r="F4" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>25</v>
+        <v>121</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -1459,60 +1481,60 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="H1" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>64</v>
-      </c>
       <c r="K1" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="E2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>69</v>
-      </c>
       <c r="G2" s="5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="H2" s="4">
         <v>1234567890</v>
@@ -1524,30 +1546,30 @@
         <v>60</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>69</v>
-      </c>
       <c r="G3" s="5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="H3" s="4">
         <v>1234567890</v>
@@ -1559,30 +1581,30 @@
         <v>90</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="E4" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F4" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>69</v>
-      </c>
       <c r="G4" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="H4" s="1">
         <v>1234567890</v>
@@ -1594,30 +1616,30 @@
         <v>30</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B5" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="F5" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>69</v>
-      </c>
       <c r="G5" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="H5" s="1">
         <v>1234567890</v>
@@ -1629,39 +1651,39 @@
         <v>60</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B6" s="6">
         <v>1234</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="K6" s="1">
         <v>1234</v>
@@ -1707,13 +1729,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -1721,7 +1743,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B2" s="1">
         <v>2</v>
@@ -1730,7 +1752,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1743,7 +1765,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1756,30 +1778,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>86</v>
-      </c>
       <c r="D2" s="11" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new scenarios code of manage artifact
</commit_message>
<xml_diff>
--- a/input-data/inputFiles/InputData.xlsx
+++ b/input-data/inputFiles/InputData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://capgemini-my.sharepoint.com/personal/abhishek-chidanand_pathrut_capgemini_com/Documents/Desktop/E2CO PROJECT/Automation/E2COAutomation/E2CO%20Automation/input-data/inputFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="57" documentId="13_ncr:1_{372006C8-C68D-43CF-8AE9-8816ABD62F43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C6500A4D-EAD1-45A2-A6CB-09800A8B03B6}"/>
+  <xr:revisionPtr revIDLastSave="90" documentId="13_ncr:1_{372006C8-C68D-43CF-8AE9-8816ABD62F43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C95C10A7-E58E-42F0-865F-77EA7C730E8A}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="7" r:id="rId1"/>
@@ -21,17 +21,28 @@
     <sheet name="Zones" sheetId="5" r:id="rId6"/>
     <sheet name="Trobleshoot" sheetId="6" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="128">
   <si>
     <t>Version</t>
   </si>
@@ -396,14 +407,32 @@
     <t>appdemo214</t>
   </si>
   <si>
-    <t>NorthZone</t>
+    <t>EastZone1</t>
+  </si>
+  <si>
+    <t>UpdateSelectRole</t>
+  </si>
+  <si>
+    <t>UpdateContactNumber</t>
+  </si>
+  <si>
+    <t>UpdateMaxInvalidAttempts</t>
+  </si>
+  <si>
+    <t>UpdateMaxValidity</t>
+  </si>
+  <si>
+    <t>UpdateUserName</t>
+  </si>
+  <si>
+    <t>deve01</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -436,6 +465,26 @@
       <color rgb="FF8F8F8F"/>
       <name val="Ubuntu"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF3E3E3E"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -474,7 +523,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -495,6 +544,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1290,8 +1345,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DC37D6C-9FD6-4975-A3E4-794B22D0C261}">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView topLeftCell="C1" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1365,16 +1420,16 @@
       <c r="F2" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="12" t="s">
         <v>121</v>
       </c>
       <c r="K2" s="10" t="s">
@@ -1403,16 +1458,16 @@
       <c r="F3" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="I3" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="12" t="s">
         <v>121</v>
       </c>
       <c r="K3" s="10" t="s">
@@ -1441,14 +1496,14 @@
       <c r="F4" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
     </row>
@@ -1461,10 +1516,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{196B5FD2-93EE-4634-85E8-41E20BCAD9A1}">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:P6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1477,9 +1532,14 @@
     <col min="9" max="9" width="18.21875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>52</v>
       </c>
@@ -1513,8 +1573,23 @@
       <c r="K1" s="1" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L1" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>62</v>
       </c>
@@ -1548,8 +1623,23 @@
       <c r="K2" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L2" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="N2" s="1">
+        <v>2334455667</v>
+      </c>
+      <c r="O2" s="1">
+        <v>4</v>
+      </c>
+      <c r="P2" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>67</v>
       </c>
@@ -1583,8 +1673,13 @@
       <c r="K3" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>62</v>
       </c>
@@ -1618,8 +1713,13 @@
       <c r="K4" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>67</v>
       </c>
@@ -1653,8 +1753,13 @@
       <c r="K5" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>90</v>
       </c>
@@ -1688,6 +1793,11 @@
       <c r="K6" s="1">
         <v>1234</v>
       </c>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
edge faulty new code
</commit_message>
<xml_diff>
--- a/input-data/inputFiles/InputData.xlsx
+++ b/input-data/inputFiles/InputData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://capgemini-my.sharepoint.com/personal/abhishek-chidanand_pathrut_capgemini_com/Documents/Desktop/E2CO PROJECT/Automation/E2COAutomation/E2CO%20Automation/input-data/inputFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="223" documentId="13_ncr:1_{372006C8-C68D-43CF-8AE9-8816ABD62F43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D7BB0A73-C5CF-4446-AA83-EBAAC37EA116}"/>
+  <xr:revisionPtr revIDLastSave="278" documentId="13_ncr:1_{372006C8-C68D-43CF-8AE9-8816ABD62F43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1791550B-4469-4818-833A-6CC6483DD498}"/>
   <bookViews>
-    <workbookView xWindow="3588" yWindow="3396" windowWidth="17280" windowHeight="8964" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="7" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="160">
   <si>
     <t>Version</t>
   </si>
@@ -243,12 +243,6 @@
     <t>developer@gmail.com</t>
   </si>
   <si>
-    <t>admin0403</t>
-  </si>
-  <si>
-    <t>dev0403</t>
-  </si>
-  <si>
     <t>versionDelete</t>
   </si>
   <si>
@@ -282,12 +276,6 @@
     <t>domainName</t>
   </si>
   <si>
-    <t>admin0703</t>
-  </si>
-  <si>
-    <t>dev0703</t>
-  </si>
-  <si>
     <t>dev0704</t>
   </si>
   <si>
@@ -505,6 +493,36 @@
   </si>
   <si>
     <t>SouthZone8</t>
+  </si>
+  <si>
+    <t>EdgeFrOOS</t>
+  </si>
+  <si>
+    <t>EdgeFrIS</t>
+  </si>
+  <si>
+    <t>CPUWarning</t>
+  </si>
+  <si>
+    <t>CPUCritical</t>
+  </si>
+  <si>
+    <t>StorageWarning</t>
+  </si>
+  <si>
+    <t>StorageCritical</t>
+  </si>
+  <si>
+    <t>MemoryWarning</t>
+  </si>
+  <si>
+    <t>MemoryCritical</t>
+  </si>
+  <si>
+    <t>GPUWarning</t>
+  </si>
+  <si>
+    <t>GPUCritical</t>
   </si>
 </sst>
 </file>
@@ -936,33 +954,33 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>62</v>
@@ -971,10 +989,10 @@
         <v>26</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>62</v>
@@ -988,7 +1006,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>62</v>
@@ -997,16 +1015,16 @@
         <v>26</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>62</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>26</v>
@@ -1014,7 +1032,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>62</v>
@@ -1023,16 +1041,16 @@
         <v>26</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>62</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>26</v>
@@ -1040,7 +1058,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>62</v>
@@ -1049,16 +1067,16 @@
         <v>26</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>62</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>26</v>
@@ -1114,7 +1132,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -1194,10 +1212,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0442710-9812-4BB8-A29F-019BB15B721A}">
-  <dimension ref="A1:V3"/>
+  <dimension ref="A1:AF3"/>
   <sheetViews>
-    <sheetView zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="V11" sqref="V11"/>
+    <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1213,9 +1231,18 @@
     <col min="18" max="18" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="14" customWidth="1"/>
     <col min="22" max="22" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="13" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="15" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="10.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1280,18 +1307,48 @@
         <v>47</v>
       </c>
       <c r="V1" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+        <v>106</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="Y1" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="Z1" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="AA1" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="AB1" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="AC1" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="AD1" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="AE1" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="AF1" s="6" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>25</v>
@@ -1348,18 +1405,48 @@
         <v>45</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+        <v>107</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="Y2" s="4">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="4">
+        <v>1</v>
+      </c>
+      <c r="AA2" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB2" s="4">
+        <v>1</v>
+      </c>
+      <c r="AC2" s="4">
+        <v>0</v>
+      </c>
+      <c r="AD2" s="4">
+        <v>1</v>
+      </c>
+      <c r="AE2" s="4">
+        <v>0</v>
+      </c>
+      <c r="AF2" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>25</v>
@@ -1416,7 +1503,33 @@
         <v>46</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
+      </c>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1"/>
+      <c r="Y3" s="4">
+        <v>80</v>
+      </c>
+      <c r="Z3" s="4">
+        <v>90</v>
+      </c>
+      <c r="AA3" s="4">
+        <v>80</v>
+      </c>
+      <c r="AB3" s="4">
+        <v>90</v>
+      </c>
+      <c r="AC3" s="4">
+        <v>80</v>
+      </c>
+      <c r="AD3" s="4">
+        <v>90</v>
+      </c>
+      <c r="AE3" s="4">
+        <v>80</v>
+      </c>
+      <c r="AF3" s="4">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1431,7 +1544,7 @@
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1445,7 +1558,7 @@
     <col min="9" max="9" width="33.77734375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="42.88671875" customWidth="1"/>
     <col min="11" max="11" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.21875" customWidth="1"/>
     <col min="13" max="13" width="26.88671875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="22.109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -1476,22 +1589,22 @@
         <v>41</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="N1" s="3" t="s">
         <v>98</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
@@ -1499,43 +1612,43 @@
         <v>42</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>43</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>44</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>127</v>
+        <v>100</v>
       </c>
       <c r="H2" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="I2" s="12" t="s">
-        <v>122</v>
+      <c r="I2" s="13" t="s">
+        <v>119</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="L2" s="11" t="s">
-        <v>127</v>
+        <v>100</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
@@ -1543,43 +1656,43 @@
         <v>42</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>43</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>44</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>127</v>
+        <v>100</v>
       </c>
       <c r="H3" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="13" t="s">
-        <v>123</v>
+      <c r="I3" s="12" t="s">
+        <v>118</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="L3" s="11" t="s">
-        <v>127</v>
+        <v>100</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
@@ -1587,50 +1700,50 @@
         <v>42</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>43</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>44</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>127</v>
+        <v>100</v>
       </c>
       <c r="H4" s="12" t="s">
         <v>26</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="L4" s="11" t="s">
-        <v>127</v>
+        <v>100</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1" display="https://hub.docker.com/_/alpine" xr:uid="{8FF599EA-A884-4513-8C3A-F070F14E4BB2}"/>
-    <hyperlink ref="J3:J4" r:id="rId2" display="https://hub.docker.com/_/alpine" xr:uid="{59C355CE-66F8-4106-83C7-D787A3796D1F}"/>
+    <hyperlink ref="J3" r:id="rId1" display="https://hub.docker.com/_/alpine" xr:uid="{8FF599EA-A884-4513-8C3A-F070F14E4BB2}"/>
+    <hyperlink ref="J2:J4" r:id="rId2" display="https://hub.docker.com/_/alpine" xr:uid="{59C355CE-66F8-4106-83C7-D787A3796D1F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId3"/>
@@ -1660,72 +1773,72 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E1" t="s">
         <v>128</v>
       </c>
-      <c r="B1" t="s">
+      <c r="F1" t="s">
         <v>129</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" t="s">
         <v>130</v>
-      </c>
-      <c r="D1" t="s">
-        <v>131</v>
-      </c>
-      <c r="E1" t="s">
-        <v>132</v>
-      </c>
-      <c r="F1" t="s">
-        <v>133</v>
-      </c>
-      <c r="G1" t="s">
-        <v>134</v>
       </c>
       <c r="H1" t="s">
         <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="J1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="K1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E2" t="s">
         <v>138</v>
       </c>
-      <c r="B2" t="s">
+      <c r="F2" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="G2" t="s">
         <v>139</v>
       </c>
-      <c r="C2" t="s">
+      <c r="H2" t="s">
+        <v>101</v>
+      </c>
+      <c r="I2" t="s">
         <v>140</v>
       </c>
-      <c r="D2" t="s">
+      <c r="J2" t="s">
+        <v>123</v>
+      </c>
+      <c r="K2" t="s">
         <v>141</v>
-      </c>
-      <c r="E2" t="s">
-        <v>142</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="G2" t="s">
-        <v>143</v>
-      </c>
-      <c r="H2" t="s">
-        <v>105</v>
-      </c>
-      <c r="I2" t="s">
-        <v>144</v>
-      </c>
-      <c r="J2" t="s">
-        <v>127</v>
-      </c>
-      <c r="K2" t="s">
-        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -1739,7 +1852,7 @@
   <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1791,22 +1904,22 @@
         <v>57</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
@@ -1823,7 +1936,7 @@
         <v>61</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>62</v>
@@ -1844,7 +1957,7 @@
         <v>26</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="M2" s="4" t="s">
         <v>64</v>
@@ -1873,7 +1986,7 @@
         <v>65</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>67</v>
+        <v>85</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>62</v>
@@ -1913,7 +2026,7 @@
         <v>61</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>62</v>
@@ -1953,7 +2066,7 @@
         <v>65</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>62</v>
@@ -1981,7 +2094,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B6" s="6">
         <v>1234</v>
@@ -1993,22 +2106,22 @@
         <v>65</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="K6" s="1">
         <v>1234</v>
@@ -2045,8 +2158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24EA177B-F3D9-4171-817C-C61F0ABB43E5}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2061,22 +2174,22 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>70</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>72</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="G1" s="6" t="s">
         <v>15</v>
@@ -2094,15 +2207,15 @@
         <v>19</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="M1" s="15" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B2" s="4">
         <v>123</v>
@@ -2111,7 +2224,7 @@
         <v>128</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E2" s="4">
         <v>10</v>
@@ -2143,7 +2256,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B3" s="4">
         <v>123</v>
@@ -2152,7 +2265,7 @@
         <v>128</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E3" s="4">
         <v>10</v>
@@ -2194,7 +2307,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2207,30 +2320,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
enterprise onboarding new code added
</commit_message>
<xml_diff>
--- a/input-data/inputFiles/InputData.xlsx
+++ b/input-data/inputFiles/InputData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://capgemini-my.sharepoint.com/personal/abhishek-chidanand_pathrut_capgemini_com/Documents/Desktop/E2CO PROJECT/Automation/E2COAutomation/E2CO%20Automation/input-data/inputFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="445" documentId="13_ncr:1_{372006C8-C68D-43CF-8AE9-8816ABD62F43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6BC2D327-B996-4C79-A815-9B1374116C86}"/>
+  <xr:revisionPtr revIDLastSave="486" documentId="13_ncr:1_{372006C8-C68D-43CF-8AE9-8816ABD62F43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F51C3BDB-1D71-4059-AED5-17C4BE2C1081}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4284" yWindow="3396" windowWidth="17280" windowHeight="8964" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="7" r:id="rId1"/>
@@ -21,10 +21,11 @@
     <sheet name="AppPolicy" sheetId="10" r:id="rId6"/>
     <sheet name="AppAffinity" sheetId="11" r:id="rId7"/>
     <sheet name="EdgePolicy" sheetId="12" r:id="rId8"/>
-    <sheet name="Reports" sheetId="8" r:id="rId9"/>
-    <sheet name="UserManagement" sheetId="4" r:id="rId10"/>
-    <sheet name="Zones" sheetId="5" r:id="rId11"/>
-    <sheet name="Trobleshoot" sheetId="6" r:id="rId12"/>
+    <sheet name="Enterprise" sheetId="13" r:id="rId9"/>
+    <sheet name="Reports" sheetId="8" r:id="rId10"/>
+    <sheet name="UserManagement" sheetId="4" r:id="rId11"/>
+    <sheet name="Zones" sheetId="5" r:id="rId12"/>
+    <sheet name="Trobleshoot" sheetId="6" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="202">
   <si>
     <t>Version</t>
   </si>
@@ -626,6 +627,33 @@
   </si>
   <si>
     <t xml:space="preserve">Resource Availability </t>
+  </si>
+  <si>
+    <t>EnterpriseName</t>
+  </si>
+  <si>
+    <t>LoginID</t>
+  </si>
+  <si>
+    <t>ConfirmPassword</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zone </t>
+  </si>
+  <si>
+    <t>CPU</t>
+  </si>
+  <si>
+    <t>Memory</t>
+  </si>
+  <si>
+    <t>Storage</t>
+  </si>
+  <si>
+    <t>Entadd</t>
+  </si>
+  <si>
+    <t>New Enterprise</t>
   </si>
 </sst>
 </file>
@@ -747,7 +775,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -791,6 +819,9 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1075,7 +1106,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1245,6 +1276,134 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0AF459C-7F6D-479A-9B78-EF3B8A70B992}">
+  <dimension ref="A1:K3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>185</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>186</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>187</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="I2" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="J2" s="19" t="s">
+        <v>161</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="C3" s="16"/>
+      <c r="D3" s="22" t="s">
+        <v>188</v>
+      </c>
+      <c r="E3" s="22" t="s">
+        <v>189</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="I3" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="J3" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="K3" s="17" t="s">
+        <v>106</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{196B5FD2-93EE-4634-85E8-41E20BCAD9A1}">
   <dimension ref="A1:P6"/>
   <sheetViews>
@@ -1551,7 +1710,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24EA177B-F3D9-4171-817C-C61F0ABB43E5}">
   <dimension ref="A1:M3"/>
   <sheetViews>
@@ -1699,7 +1858,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45558A6E-173A-4774-B294-BD2BB2951523}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1857,7 +2016,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0442710-9812-4BB8-A29F-019BB15B721A}">
   <dimension ref="A1:AF3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+    <sheetView zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
       <selection activeCell="Y12" sqref="Y12"/>
     </sheetView>
   </sheetViews>
@@ -2650,129 +2809,93 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0AF459C-7F6D-479A-9B78-EF3B8A70B992}">
-  <dimension ref="A1:K3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{722A60C4-D262-4C3E-8327-F7A9807FEADF}">
+  <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>130</v>
-      </c>
+      <c r="A1" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="K1" s="23"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>192</v>
-      </c>
-      <c r="C2" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="D2" s="19" t="s">
-        <v>185</v>
-      </c>
-      <c r="E2" s="19" t="s">
-        <v>186</v>
-      </c>
-      <c r="F2" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="G2" s="19" t="s">
-        <v>187</v>
-      </c>
-      <c r="H2" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="I2" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="J2" s="19" t="s">
-        <v>161</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="17" t="s">
-        <v>183</v>
-      </c>
-      <c r="B3" s="18" t="s">
-        <v>184</v>
-      </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="22" t="s">
-        <v>188</v>
-      </c>
-      <c r="E3" s="22" t="s">
-        <v>189</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="I3" s="17" t="s">
-        <v>132</v>
-      </c>
-      <c r="J3" s="17" t="s">
+      <c r="A2" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="K3" s="17" t="s">
-        <v>106</v>
-      </c>
+      <c r="H2" s="4">
+        <v>1</v>
+      </c>
+      <c r="I2" s="4">
+        <v>1</v>
+      </c>
+      <c r="J2" s="4">
+        <v>1</v>
+      </c>
+      <c r="K2" s="23"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{AECEA959-0E1D-4D9A-ADC4-220EEF4B84EF}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{75779DDB-5D4B-464A-89FE-4124CC541DED}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
sdk scenarios merged code
</commit_message>
<xml_diff>
--- a/input-data/inputFiles/InputData.xlsx
+++ b/input-data/inputFiles/InputData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://capgemini-my.sharepoint.com/personal/abhishek-chidanand_pathrut_capgemini_com/Documents/Desktop/E2CO PROJECT/Automation/E2COAutomation/E2CO%20Automation/input-data/inputFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="486" documentId="13_ncr:1_{372006C8-C68D-43CF-8AE9-8816ABD62F43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F51C3BDB-1D71-4059-AED5-17C4BE2C1081}"/>
+  <xr:revisionPtr revIDLastSave="509" documentId="13_ncr:1_{372006C8-C68D-43CF-8AE9-8816ABD62F43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6D229286-D335-4486-89E2-AF56C4B6A614}"/>
   <bookViews>
-    <workbookView xWindow="4284" yWindow="3396" windowWidth="17280" windowHeight="8964" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="7" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="201">
   <si>
     <t>Version</t>
   </si>
@@ -248,9 +248,6 @@
     <t>versionDelete</t>
   </si>
   <si>
-    <t>artifact0304</t>
-  </si>
-  <si>
     <t>zoneid</t>
   </si>
   <si>
@@ -338,30 +335,15 @@
     <t>ApplicationNameFrDeProvision</t>
   </si>
   <si>
-    <t>artifact0310</t>
-  </si>
-  <si>
     <t>ApplicationNmFrDeboard</t>
   </si>
   <si>
-    <t>artifact0311</t>
-  </si>
-  <si>
     <t>EastZone</t>
   </si>
   <si>
     <t>IN</t>
   </si>
   <si>
-    <t>marioapp0005</t>
-  </si>
-  <si>
-    <t>64813a8d2000005</t>
-  </si>
-  <si>
-    <t>f6480bac6c000010</t>
-  </si>
-  <si>
     <t>alpine</t>
   </si>
   <si>
@@ -392,9 +374,6 @@
     <t>UpdateUserName</t>
   </si>
   <si>
-    <t>deve01</t>
-  </si>
-  <si>
     <t>ImageTag</t>
   </si>
   <si>
@@ -654,13 +633,31 @@
   </si>
   <si>
     <t>New Enterprise</t>
+  </si>
+  <si>
+    <t>artifact3003</t>
+  </si>
+  <si>
+    <t>artifact3004</t>
+  </si>
+  <si>
+    <t>artifact3005</t>
+  </si>
+  <si>
+    <t>alpineapp123</t>
+  </si>
+  <si>
+    <t>64d22e67900000b</t>
+  </si>
+  <si>
+    <t>c64b97290e000011</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -681,12 +678,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF8F8F8F"/>
-      <name val="Ubuntu"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -775,7 +766,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -795,30 +786,29 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1106,7 +1096,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1123,33 +1113,33 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>82</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>61</v>
@@ -1158,16 +1148,16 @@
         <v>26</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>61</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>61</v>
+        <v>90</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>26</v>
@@ -1175,7 +1165,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>61</v>
@@ -1184,16 +1174,16 @@
         <v>26</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>61</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>26</v>
@@ -1201,7 +1191,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>61</v>
@@ -1210,16 +1200,16 @@
         <v>26</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>61</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>26</v>
@@ -1227,7 +1217,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>61</v>
@@ -1236,16 +1226,16 @@
         <v>26</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>61</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>26</v>
@@ -1298,103 +1288,103 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>192</v>
-      </c>
-      <c r="C2" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="D2" s="19" t="s">
+        <v>184</v>
+      </c>
+      <c r="B2" s="17" t="s">
         <v>185</v>
       </c>
-      <c r="E2" s="19" t="s">
-        <v>186</v>
-      </c>
-      <c r="F2" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="G2" s="19" t="s">
-        <v>187</v>
-      </c>
-      <c r="H2" s="16" t="s">
+      <c r="C2" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="J2" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="C3" s="15"/>
+      <c r="D3" s="21" t="s">
+        <v>181</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>182</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="I3" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="J3" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="K3" s="16" t="s">
         <v>100</v>
-      </c>
-      <c r="I2" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="J2" s="19" t="s">
-        <v>161</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="17" t="s">
-        <v>183</v>
-      </c>
-      <c r="B3" s="18" t="s">
-        <v>184</v>
-      </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="22" t="s">
-        <v>188</v>
-      </c>
-      <c r="E3" s="22" t="s">
-        <v>189</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="I3" s="17" t="s">
-        <v>132</v>
-      </c>
-      <c r="J3" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="K3" s="17" t="s">
-        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -1408,7 +1398,7 @@
   <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1460,22 +1450,22 @@
         <v>56</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
@@ -1492,7 +1482,7 @@
         <v>60</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>61</v>
@@ -1513,7 +1503,7 @@
         <v>26</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>114</v>
+        <v>84</v>
       </c>
       <c r="M2" s="4" t="s">
         <v>63</v>
@@ -1542,7 +1532,7 @@
         <v>64</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>61</v>
@@ -1582,7 +1572,7 @@
         <v>60</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>61</v>
@@ -1622,7 +1612,7 @@
         <v>64</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>61</v>
@@ -1650,7 +1640,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B6" s="6">
         <v>1234</v>
@@ -1662,22 +1652,22 @@
         <v>64</v>
       </c>
       <c r="E6" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>77</v>
-      </c>
       <c r="I6" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K6" s="1">
         <v>1234</v>
@@ -1730,22 +1720,22 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>68</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>69</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="14" t="s">
-        <v>136</v>
+      <c r="E1" s="13" t="s">
+        <v>129</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="G1" s="6" t="s">
         <v>15</v>
@@ -1763,15 +1753,15 @@
         <v>19</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="M1" s="14" t="s">
-        <v>139</v>
+        <v>131</v>
+      </c>
+      <c r="M1" s="13" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="B2" s="4">
         <v>123</v>
@@ -1780,7 +1770,7 @@
         <v>128</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="E2" s="4">
         <v>10</v>
@@ -1794,7 +1784,7 @@
       <c r="H2" s="4">
         <v>404</v>
       </c>
-      <c r="I2" s="15" t="s">
+      <c r="I2" s="14" t="s">
         <v>32</v>
       </c>
       <c r="J2" s="4">
@@ -1812,7 +1802,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="B3" s="4">
         <v>123</v>
@@ -1821,7 +1811,7 @@
         <v>128</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="E3" s="4">
         <v>10</v>
@@ -1835,7 +1825,7 @@
       <c r="H3" s="4">
         <v>404</v>
       </c>
-      <c r="I3" s="15" t="s">
+      <c r="I3" s="14" t="s">
         <v>32</v>
       </c>
       <c r="J3" s="4">
@@ -1863,7 +1853,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1876,30 +1866,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="C2" s="19" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>102</v>
+      <c r="D2" s="15" t="s">
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -2017,7 +2007,7 @@
   <dimension ref="A1:AF3"/>
   <sheetViews>
     <sheetView zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="Y12" sqref="Y12"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2030,7 +2020,7 @@
     <col min="8" max="8" width="9.77734375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.88671875" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="14" customWidth="1"/>
     <col min="22" max="22" width="13.21875" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="10.109375" bestFit="1" customWidth="1"/>
@@ -2109,48 +2099,48 @@
         <v>46</v>
       </c>
       <c r="V1" s="3" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="W1" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="Y1" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="Z1" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="AA1" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="AB1" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="AC1" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="AD1" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="AE1" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="Y1" s="6" t="s">
+      <c r="AF1" s="6" t="s">
         <v>143</v>
-      </c>
-      <c r="Z1" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="AA1" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="AB1" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="AC1" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="AD1" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="AE1" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="AF1" s="6" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>25</v>
@@ -2195,7 +2185,7 @@
         <v>2</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="S2" s="1">
         <v>12.4168</v>
@@ -2207,13 +2197,13 @@
         <v>44</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="Y2" s="4">
         <v>0</v>
@@ -2245,10 +2235,10 @@
         <v>45</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>25</v>
@@ -2305,7 +2295,7 @@
         <v>45</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="W3" s="1"/>
       <c r="X3" s="1"/>
@@ -2345,8 +2335,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DC37D6C-9FD6-4975-A3E4-794B22D0C261}">
   <dimension ref="A1:V4"/>
   <sheetViews>
-    <sheetView zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
-      <selection activeCell="T9" sqref="T9"/>
+    <sheetView tabSelected="1" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2388,10 +2378,10 @@
         <v>37</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>38</v>
@@ -2406,40 +2396,40 @@
         <v>40</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="N1" s="4" t="s">
         <v>51</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="Q1" s="4" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="R1" s="4" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="S1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="T1" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="3" t="s">
         <v>95</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.3">
@@ -2447,40 +2437,40 @@
         <v>41</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>96</v>
+        <v>195</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>42</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>96</v>
+        <v>195</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>96</v>
+        <v>195</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I2" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="J2" s="12" t="s">
+      <c r="I2" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="J2" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="K2" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="L2" s="13" t="s">
-        <v>118</v>
+      <c r="K2" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="L2" s="12" t="s">
+        <v>111</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="N2" s="5"/>
       <c r="O2" s="1"/>
@@ -2488,16 +2478,16 @@
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
       <c r="S2" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="T2" s="11" t="s">
-        <v>161</v>
+        <v>102</v>
+      </c>
+      <c r="T2" s="10" t="s">
+        <v>96</v>
       </c>
       <c r="U2" s="4" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="V2" s="4" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.3">
@@ -2505,38 +2495,38 @@
         <v>41</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>98</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>104</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>42</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>98</v>
+        <v>196</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>98</v>
+        <v>196</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I3" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="J3" s="12" t="s">
+      <c r="I3" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="J3" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12" t="s">
-        <v>117</v>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11" t="s">
+        <v>110</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
@@ -2544,51 +2534,55 @@
       <c r="Q3" s="5"/>
       <c r="R3" s="5"/>
       <c r="S3" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="T3" s="11" t="s">
-        <v>161</v>
+        <v>113</v>
+      </c>
+      <c r="T3" s="10" t="s">
+        <v>96</v>
       </c>
       <c r="U3" s="4" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="V3" s="4" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>66</v>
+        <v>197</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
+        <v>146</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>197</v>
+      </c>
       <c r="G4" s="4" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I4" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="J4" s="12" t="s">
+      <c r="I4" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="J4" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12" t="s">
-        <v>119</v>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11" t="s">
+        <v>112</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="N4" s="5" t="s">
         <v>57</v>
@@ -2600,22 +2594,22 @@
         <v>61</v>
       </c>
       <c r="Q4" s="5" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="R4" s="5">
         <v>20</v>
       </c>
       <c r="S4" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="T4" s="11" t="s">
-        <v>161</v>
+        <v>114</v>
+      </c>
+      <c r="T4" s="10" t="s">
+        <v>96</v>
       </c>
       <c r="U4" s="4" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="V4" s="4" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -2646,12 +2640,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="16" t="s">
-        <v>180</v>
+      <c r="A2" s="15" t="s">
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -2678,27 +2672,27 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="16" t="s">
-        <v>108</v>
+      <c r="A2" s="15" t="s">
+        <v>102</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="D2" s="4">
         <v>5</v>
@@ -2727,30 +2721,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="B1" s="4" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="16" t="s">
-        <v>108</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>171</v>
-      </c>
       <c r="C2" s="4" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -2777,27 +2771,27 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="D2" s="4">
         <v>10</v>
@@ -2812,7 +2806,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{722A60C4-D262-4C3E-8327-F7A9807FEADF}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
@@ -2827,46 +2821,46 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>11</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="K1" s="23"/>
+        <v>192</v>
+      </c>
+      <c r="K1" s="22"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>61</v>
@@ -2875,10 +2869,10 @@
         <v>61</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H2" s="4">
         <v>1</v>
@@ -2889,7 +2883,7 @@
       <c r="J2" s="4">
         <v>1</v>
       </c>
-      <c r="K2" s="23"/>
+      <c r="K2" s="22"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
code modified in excel sheet
</commit_message>
<xml_diff>
--- a/input-data/inputFiles/InputData.xlsx
+++ b/input-data/inputFiles/InputData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://capgemini-my.sharepoint.com/personal/abhishek-chidanand_pathrut_capgemini_com/Documents/Desktop/E2CO PROJECT/Automation/E2COAutomation/E2CO%20Automation/input-data/inputFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="538" documentId="13_ncr:1_{372006C8-C68D-43CF-8AE9-8816ABD62F43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{98F7EB09-5225-4526-A30D-13DF769AC14F}"/>
+  <xr:revisionPtr revIDLastSave="568" documentId="13_ncr:1_{372006C8-C68D-43CF-8AE9-8816ABD62F43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E251057-78C0-492A-A62F-496408598416}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="7" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="207">
   <si>
     <t>Version</t>
   </si>
@@ -182,12 +182,6 @@
     <t>low</t>
   </si>
   <si>
-    <t>edge035</t>
-  </si>
-  <si>
-    <t>edge038</t>
-  </si>
-  <si>
     <t>EdgeIdDeboard</t>
   </si>
   <si>
@@ -644,15 +638,6 @@
     <t>artifact3005</t>
   </si>
   <si>
-    <t>alpineapp123</t>
-  </si>
-  <si>
-    <t>64d22e67900000b</t>
-  </si>
-  <si>
-    <t>c64b97290e000011</t>
-  </si>
-  <si>
     <t>NorthZone</t>
   </si>
   <si>
@@ -669,13 +654,28 @@
   </si>
   <si>
     <t>ec_client-sdk_Android_12345.zip</t>
+  </si>
+  <si>
+    <t>l6502d86d6000008</t>
+  </si>
+  <si>
+    <t>6502d9ff7000008</t>
+  </si>
+  <si>
+    <t>SouthZone9</t>
+  </si>
+  <si>
+    <t>edge28</t>
+  </si>
+  <si>
+    <t>edge29</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -734,6 +734,12 @@
       <name val="Ubuntu"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF8F8F8F"/>
+      <name val="Ubuntu"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -784,7 +790,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -830,6 +836,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1131,51 +1138,51 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>81</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>26</v>
@@ -1183,25 +1190,25 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>26</v>
@@ -1209,25 +1216,25 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>26</v>
@@ -1235,25 +1242,25 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>26</v>
@@ -1306,103 +1313,103 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>120</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D2" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="G2" s="18" t="s">
         <v>178</v>
       </c>
-      <c r="E2" s="18" t="s">
-        <v>179</v>
-      </c>
-      <c r="F2" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="G2" s="18" t="s">
-        <v>180</v>
-      </c>
       <c r="H2" s="15" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="I2" s="15" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="J2" s="18" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C3" s="15"/>
       <c r="D3" s="21" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="16" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="I3" s="16" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="J3" s="16" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="K3" s="16" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1439,84 +1446,84 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="I1" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>56</v>
-      </c>
       <c r="K1" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="M1" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="O1" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="P1" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="O1" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>106</v>
-      </c>
       <c r="Q1" s="6" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="R1" s="6" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="S1" s="6" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="D2" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="E2" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>61</v>
-      </c>
       <c r="G2" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H2" s="4">
         <v>1234567890</v>
@@ -1531,10 +1538,10 @@
         <v>26</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="N2" s="4">
         <v>2334455667</v>
@@ -1546,36 +1553,36 @@
         <v>60</v>
       </c>
       <c r="Q2" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="S2" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>64</v>
-      </c>
       <c r="E3" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H3" s="4">
         <v>1234567890</v>
@@ -1600,25 +1607,25 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="D4" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="E4" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="F4" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>61</v>
-      </c>
       <c r="G4" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H4" s="1">
         <v>1234567890</v>
@@ -1643,25 +1650,25 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>64</v>
-      </c>
       <c r="E5" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H5" s="1">
         <v>1234567890</v>
@@ -1686,34 +1693,34 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B6" s="6">
         <v>1234</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E6" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>77</v>
-      </c>
       <c r="G6" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K6" s="1">
         <v>1234</v>
@@ -1751,10 +1758,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24EA177B-F3D9-4171-817C-C61F0ABB43E5}">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1769,22 +1776,22 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>66</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>68</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G1" s="6" t="s">
         <v>15</v>
@@ -1802,15 +1809,15 @@
         <v>19</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="M1" s="13" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B2" s="4">
         <v>123</v>
@@ -1819,7 +1826,7 @@
         <v>128</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E2" s="4">
         <v>10</v>
@@ -1851,7 +1858,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B3" s="4">
         <v>123</v>
@@ -1860,7 +1867,7 @@
         <v>128</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E3" s="4">
         <v>10</v>
@@ -1887,6 +1894,47 @@
         <v>21</v>
       </c>
       <c r="M3" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="B4" s="4">
+        <v>123</v>
+      </c>
+      <c r="C4" s="4">
+        <v>128</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="E4" s="4">
+        <v>10</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" s="4">
+        <v>405</v>
+      </c>
+      <c r="I4" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="J4" s="4">
+        <v>1</v>
+      </c>
+      <c r="K4" s="4">
+        <v>2</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M4" s="4">
         <v>1</v>
       </c>
     </row>
@@ -1902,7 +1950,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1915,30 +1963,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>202</v>
+      </c>
+      <c r="C2" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="15" t="s">
-        <v>198</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>200</v>
-      </c>
-      <c r="C2" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>199</v>
+      <c r="D2" s="23" t="s">
+        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -1951,7 +1999,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
@@ -1974,10 +2022,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -1994,7 +2042,7 @@
         <v>12345</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -2066,8 +2114,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0442710-9812-4BB8-A29F-019BB15B721A}">
   <dimension ref="A1:AF3"/>
   <sheetViews>
-    <sheetView zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="Z36" sqref="Z36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2156,51 +2204,51 @@
         <v>24</v>
       </c>
       <c r="U1" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="V1" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="W1" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="Y1" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Z1" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="Y1" s="6" t="s">
+      <c r="AA1" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="Z1" s="6" t="s">
+      <c r="AB1" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="AA1" s="6" t="s">
+      <c r="AC1" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="AB1" s="6" t="s">
+      <c r="AD1" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="AC1" s="6" t="s">
+      <c r="AE1" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="AD1" s="6" t="s">
+      <c r="AF1" s="6" t="s">
         <v>141</v>
-      </c>
-      <c r="AE1" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="AF1" s="6" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>154</v>
+        <v>205</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>196</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>25</v>
@@ -2245,7 +2293,7 @@
         <v>2</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="S2" s="1">
         <v>12.4168</v>
@@ -2254,16 +2302,16 @@
         <v>-34.703800000000001</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>44</v>
+        <v>205</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>100</v>
+        <v>172</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>100</v>
+        <v>172</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>100</v>
+        <v>172</v>
       </c>
       <c r="Y2" s="4">
         <v>0</v>
@@ -2292,13 +2340,13 @@
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>96</v>
+        <v>206</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>196</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>25</v>
@@ -2352,10 +2400,10 @@
         <v>-34.703800000000001</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>45</v>
+        <v>206</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="W3" s="1"/>
       <c r="X3" s="1"/>
@@ -2396,7 +2444,7 @@
   <dimension ref="A1:V4"/>
   <sheetViews>
     <sheetView zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2438,10 +2486,10 @@
         <v>37</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>38</v>
@@ -2456,40 +2504,40 @@
         <v>40</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="O1" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="Q1" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="Q1" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>150</v>
-      </c>
       <c r="S1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="V1" s="3" t="s">
         <v>93</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.3">
@@ -2497,40 +2545,40 @@
         <v>41</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>42</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>43</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>96</v>
+        <v>196</v>
       </c>
       <c r="J2" s="11" t="s">
         <v>26</v>
       </c>
       <c r="K2" s="13" t="s">
-        <v>100</v>
+        <v>172</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="N2" s="5"/>
       <c r="O2" s="1"/>
@@ -2538,16 +2586,16 @@
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
       <c r="S2" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="T2" s="10" t="s">
-        <v>96</v>
+        <v>196</v>
       </c>
       <c r="U2" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="V2" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.3">
@@ -2555,38 +2603,38 @@
         <v>41</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>42</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>43</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>96</v>
+        <v>196</v>
       </c>
       <c r="J3" s="11" t="s">
         <v>26</v>
       </c>
       <c r="K3" s="11"/>
       <c r="L3" s="11" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
@@ -2594,82 +2642,82 @@
       <c r="Q3" s="5"/>
       <c r="R3" s="5"/>
       <c r="S3" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="T3" s="10" t="s">
-        <v>96</v>
+        <v>196</v>
       </c>
       <c r="U3" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="V3" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>146</v>
-      </c>
       <c r="E4" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>43</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>96</v>
+        <v>196</v>
       </c>
       <c r="J4" s="11" t="s">
         <v>26</v>
       </c>
       <c r="K4" s="11"/>
       <c r="L4" s="11" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="O4" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="P4" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="Q4" s="5" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="R4" s="5">
         <v>20</v>
       </c>
       <c r="S4" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="T4" s="10" t="s">
-        <v>96</v>
+        <v>196</v>
       </c>
       <c r="U4" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="V4" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -2700,12 +2748,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -2732,27 +2780,27 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>157</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D2" s="4">
         <v>5</v>
@@ -2781,30 +2829,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -2831,27 +2879,27 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>167</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>170</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>172</v>
       </c>
       <c r="D2" s="4">
         <v>10</v>
@@ -2882,58 +2930,58 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>186</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>11</v>
       </c>
       <c r="G1" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>190</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>192</v>
       </c>
       <c r="K1" s="22"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="H2" s="4">
         <v>1</v>

</xml_diff>

<commit_message>
Code modified for dev status of app
</commit_message>
<xml_diff>
--- a/input-data/inputFiles/InputData.xlsx
+++ b/input-data/inputFiles/InputData.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="568" documentId="13_ncr:1_{372006C8-C68D-43CF-8AE9-8816ABD62F43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E251057-78C0-492A-A62F-496408598416}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="7" r:id="rId1"/>
@@ -2114,7 +2114,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0442710-9812-4BB8-A29F-019BB15B721A}">
   <dimension ref="A1:AF3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+    <sheetView topLeftCell="H1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
       <selection activeCell="Z36" sqref="Z36"/>
     </sheetView>
   </sheetViews>
@@ -2443,7 +2443,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DC37D6C-9FD6-4975-A3E4-794B22D0C261}">
   <dimension ref="A1:V4"/>
   <sheetViews>
-    <sheetView zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
VM application onboarding code modified
</commit_message>
<xml_diff>
--- a/input-data/inputFiles/InputData.xlsx
+++ b/input-data/inputFiles/InputData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://capgemini-my.sharepoint.com/personal/abhishek-chidanand_pathrut_capgemini_com/Documents/Desktop/E2CO PROJECT/Automation/E2COAutomation/E2CO%20Automation/input-data/inputFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="568" documentId="13_ncr:1_{372006C8-C68D-43CF-8AE9-8816ABD62F43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E251057-78C0-492A-A62F-496408598416}"/>
+  <xr:revisionPtr revIDLastSave="586" documentId="13_ncr:1_{372006C8-C68D-43CF-8AE9-8816ABD62F43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C0FD9F2C-A10E-464E-B568-B7B97E940A23}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -494,9 +494,6 @@
     <t>sshkey</t>
   </si>
   <si>
-    <t>ephermalvolume</t>
-  </si>
-  <si>
     <t>abc123</t>
   </si>
   <si>
@@ -566,9 +563,6 @@
     <t xml:space="preserve">appdemo214-w64ba19ff400000f </t>
   </si>
   <si>
-    <t>edge3</t>
-  </si>
-  <si>
     <t>clusterthree</t>
   </si>
   <si>
@@ -638,9 +632,6 @@
     <t>artifact3005</t>
   </si>
   <si>
-    <t>NorthZone</t>
-  </si>
-  <si>
     <t>UserNameFrDelete</t>
   </si>
   <si>
@@ -669,6 +660,15 @@
   </si>
   <si>
     <t>edge29</t>
+  </si>
+  <si>
+    <t>edge6</t>
+  </si>
+  <si>
+    <t>edge5</t>
+  </si>
+  <si>
+    <t>ephermalVolume</t>
   </si>
 </sst>
 </file>
@@ -790,7 +790,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -837,6 +837,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1313,7 +1316,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>113</v>
@@ -1348,25 +1351,25 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C2" s="20" t="s">
         <v>122</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F2" s="19" t="s">
         <v>71</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H2" s="15" t="s">
         <v>95</v>
@@ -1375,7 +1378,7 @@
         <v>123</v>
       </c>
       <c r="J2" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>99</v>
@@ -1383,17 +1386,17 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C3" s="15"/>
       <c r="D3" s="21" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>71</v>
@@ -1494,13 +1497,13 @@
         <v>104</v>
       </c>
       <c r="Q1" s="6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="R1" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="S1" s="6" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
@@ -1899,7 +1902,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B4" s="4">
         <v>123</v>
@@ -1980,13 +1983,13 @@
         <v>100</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C2" s="19" t="s">
         <v>71</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -2025,7 +2028,7 @@
         <v>63</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -2042,7 +2045,7 @@
         <v>12345</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -2114,8 +2117,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0442710-9812-4BB8-A29F-019BB15B721A}">
   <dimension ref="A1:AF3"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="Z36" sqref="Z36"/>
+    <sheetView zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2242,10 +2245,10 @@
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>196</v>
+        <v>94</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>95</v>
@@ -2293,7 +2296,7 @@
         <v>2</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="S2" s="1">
         <v>12.4168</v>
@@ -2302,16 +2305,16 @@
         <v>-34.703800000000001</v>
       </c>
       <c r="U2" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="V2" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="V2" s="1" t="s">
-        <v>172</v>
-      </c>
       <c r="W2" s="1" t="s">
-        <v>172</v>
+        <v>205</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>172</v>
+        <v>205</v>
       </c>
       <c r="Y2" s="4">
         <v>0</v>
@@ -2340,10 +2343,10 @@
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>196</v>
+        <v>94</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>95</v>
@@ -2400,10 +2403,10 @@
         <v>-34.703800000000001</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>99</v>
+        <v>204</v>
       </c>
       <c r="W3" s="1"/>
       <c r="X3" s="1"/>
@@ -2443,8 +2446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DC37D6C-9FD6-4975-A3E4-794B22D0C261}">
   <dimension ref="A1:V4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
+      <selection activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2486,10 +2489,10 @@
         <v>37</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>38</v>
@@ -2525,7 +2528,7 @@
         <v>147</v>
       </c>
       <c r="R1" s="4" t="s">
-        <v>148</v>
+        <v>206</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>91</v>
@@ -2545,7 +2548,7 @@
         <v>41</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>96</v>
@@ -2554,10 +2557,10 @@
         <v>42</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>100</v>
@@ -2565,14 +2568,14 @@
       <c r="H2" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I2" s="10" t="s">
-        <v>196</v>
+      <c r="I2" s="15" t="s">
+        <v>94</v>
       </c>
       <c r="J2" s="11" t="s">
         <v>26</v>
       </c>
       <c r="K2" s="13" t="s">
-        <v>172</v>
+        <v>205</v>
       </c>
       <c r="L2" s="12" t="s">
         <v>109</v>
@@ -2588,8 +2591,8 @@
       <c r="S2" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="T2" s="10" t="s">
-        <v>196</v>
+      <c r="T2" s="15" t="s">
+        <v>94</v>
       </c>
       <c r="U2" s="4" t="s">
         <v>100</v>
@@ -2603,7 +2606,7 @@
         <v>41</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>96</v>
@@ -2612,10 +2615,10 @@
         <v>42</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>111</v>
@@ -2623,8 +2626,8 @@
       <c r="H3" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I3" s="10" t="s">
-        <v>196</v>
+      <c r="I3" s="15" t="s">
+        <v>94</v>
       </c>
       <c r="J3" s="11" t="s">
         <v>26</v>
@@ -2644,8 +2647,8 @@
       <c r="S3" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="T3" s="10" t="s">
-        <v>196</v>
+      <c r="T3" s="15" t="s">
+        <v>94</v>
       </c>
       <c r="U3" s="4" t="s">
         <v>111</v>
@@ -2659,7 +2662,7 @@
         <v>142</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>143</v>
@@ -2668,10 +2671,10 @@
         <v>144</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>112</v>
@@ -2679,8 +2682,8 @@
       <c r="H4" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I4" s="10" t="s">
-        <v>196</v>
+      <c r="I4" s="15" t="s">
+        <v>94</v>
       </c>
       <c r="J4" s="11" t="s">
         <v>26</v>
@@ -2702,16 +2705,16 @@
         <v>59</v>
       </c>
       <c r="Q4" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="R4" s="5">
-        <v>20</v>
+        <v>148</v>
+      </c>
+      <c r="R4" s="24">
+        <v>10</v>
       </c>
       <c r="S4" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="T4" s="10" t="s">
-        <v>196</v>
+      <c r="T4" s="15" t="s">
+        <v>94</v>
       </c>
       <c r="U4" s="4" t="s">
         <v>112</v>
@@ -2748,12 +2751,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -2780,16 +2783,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>156</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -2797,10 +2800,10 @@
         <v>100</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>158</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>159</v>
       </c>
       <c r="D2" s="4">
         <v>5</v>
@@ -2829,16 +2832,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>155</v>
-      </c>
       <c r="C1" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>160</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -2846,10 +2849,10 @@
         <v>100</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>162</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>163</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>94</v>
@@ -2879,27 +2882,27 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>166</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>169</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>170</v>
       </c>
       <c r="D2" s="4">
         <v>10</v>
@@ -2915,7 +2918,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2930,46 +2933,46 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>79</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>78</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>11</v>
       </c>
       <c r="G1" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>188</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>190</v>
       </c>
       <c r="K1" s="22"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>59</v>
@@ -2978,10 +2981,10 @@
         <v>59</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>196</v>
+        <v>94</v>
       </c>
       <c r="H2" s="4">
         <v>1</v>

</xml_diff>